<commit_message>
test first architecture completed
</commit_message>
<xml_diff>
--- a/AZURE_xlsx/Azure-go-metrics.xlsx
+++ b/AZURE_xlsx/Azure-go-metrics.xlsx
@@ -3,10 +3,10 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Somma Requests per DDI-first-ar" sheetId="1" r:id="rId1"/>
-    <sheet name="Media Response Time per DDI-fir" sheetId="2" r:id="rId2"/>
-    <sheet name="Min Response Time per DDI-first" sheetId="3" r:id="rId3"/>
-    <sheet name="Max Response Time per DDI-first" sheetId="4" r:id="rId4"/>
+    <sheet name="Sum Requests for DDI-first-arch" sheetId="1" r:id="rId1"/>
+    <sheet name="Min Response Time for DDI-first" sheetId="2" r:id="rId2"/>
+    <sheet name="Avg Response Time for DDI-first" sheetId="3" r:id="rId3"/>
+    <sheet name="Max Response Time for DDI-first" sheetId="4" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -433,7 +433,7 @@
         <v xml:space="preserve">Chart Title: </v>
       </c>
       <c r="B1" t="str">
-        <v>Somma Requests per DDI-first-architecture-go3</v>
+        <v>Sum Requests for DDI-first-architecture-go3</v>
       </c>
     </row>
     <row r="2">
@@ -443,22 +443,22 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Sat Sep 07 2024 18:35:42 GMT+0200 (Ora legale dell’Europa centrale)</v>
+        <v>Thu Sep 26 2024 01:03:21 GMT+0200 (Ora legale dell’Europa centrale)</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Sat Sep 07 2024 18:44:13 GMT+0200 (Ora legale dell’Europa centrale)</v>
+        <v>Thu Sep 26 2024 01:13:11 GMT+0200 (Ora legale dell’Europa centrale)</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Grain: Automatica</v>
+        <v>Grain: Automatic</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>Aggregation type: Somma</v>
+        <v>Aggregation type: Sum</v>
       </c>
     </row>
     <row r="7">
@@ -486,76 +486,76 @@
         <v/>
       </c>
       <c r="B11" t="str">
-        <v>DDI-first-architecture-go3, Requests (Somma), DDI-first-architecture-go3</v>
+        <v>DDI-first-architecture-go3, Requests (Sum), DDI-first-architecture-go3</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>45542.775</v>
+        <v>45561.044444444444</v>
       </c>
       <c r="B12">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>45542.77569444444</v>
+        <v>45561.04513888889</v>
       </c>
       <c r="B13">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>45542.77638888889</v>
+        <v>45561.04583333333</v>
       </c>
       <c r="B14">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>45542.777083333334</v>
+        <v>45561.04652777778</v>
       </c>
       <c r="B15">
-        <v>158</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>45542.77777777778</v>
+        <v>45561.04722222222</v>
       </c>
       <c r="B16">
-        <v>538</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>45542.77847222222</v>
+        <v>45561.04791666667</v>
       </c>
       <c r="B17">
-        <v>131</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>45542.77916666667</v>
+        <v>45561.04861111111</v>
       </c>
       <c r="B18">
-        <v>21</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>45542.779861111114</v>
+        <v>45561.049305555556</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>45542.78055555555</v>
+        <v>45561.05</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -569,157 +569,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <cols>
-    <col min="1" max="1" customWidth="1" width="15"/>
-    <col min="2" max="2" customWidth="1" width="11"/>
-    <col min="3" max="3" customWidth="1" width="11"/>
-    <col min="4" max="4" customWidth="1" width="11"/>
-    <col min="5" max="5" customWidth="1" width="11"/>
-    <col min="6" max="6" customWidth="1" width="11"/>
-    <col min="7" max="7" customWidth="1" width="11"/>
-    <col min="8" max="8" customWidth="1" width="11"/>
-    <col min="9" max="9" customWidth="1" width="11"/>
-    <col min="10" max="10" customWidth="1" width="11"/>
-    <col min="11" max="11" customWidth="1" width="11"/>
-    <col min="12" max="12" customWidth="1" width="11"/>
-    <col min="13" max="13" customWidth="1" width="11"/>
-    <col min="14" max="14" customWidth="1" width="11"/>
-    <col min="15" max="15" customWidth="1" width="11"/>
-    <col min="16" max="16" customWidth="1" width="11"/>
-    <col min="17" max="17" customWidth="1" width="11"/>
-    <col min="18" max="18" customWidth="1" width="11"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v xml:space="preserve">Chart Title: </v>
-      </c>
-      <c r="B1" t="str">
-        <v>Media Response Time per DDI-first-architecture-go3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>Sat Sep 07 2024 18:35:42 GMT+0200 (Ora legale dell’Europa centrale)</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>Sat Sep 07 2024 18:44:13 GMT+0200 (Ora legale dell’Europa centrale)</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>Grain: Automatica</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Aggregation type: Media</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>Grouping: None</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>Filters: None</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>Chart type: Line</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v/>
-      </c>
-      <c r="B11" t="str">
-        <v>DDI-first-architecture-go3, Response Time (Media), DDI-first-architecture-go3</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1">
-        <v>45542.775</v>
-      </c>
-      <c r="B12">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1">
-        <v>45542.77569444444</v>
-      </c>
-      <c r="B13">
-        <v>0.07151515151515152</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1">
-        <v>45542.77638888889</v>
-      </c>
-      <c r="B14">
-        <v>0.051739495798319324</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1">
-        <v>45542.777083333334</v>
-      </c>
-      <c r="B15">
-        <v>0.04596202531645569</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1">
-        <v>45542.77777777778</v>
-      </c>
-      <c r="B16">
-        <v>0.05428810408921933</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1">
-        <v>45542.77847222222</v>
-      </c>
-      <c r="B17">
-        <v>0.04990839694656488</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1">
-        <v>45542.77916666667</v>
-      </c>
-      <c r="B18">
-        <v>0.053285714285714283</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B18"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -753,7 +602,7 @@
         <v xml:space="preserve">Chart Title: </v>
       </c>
       <c r="B1" t="str">
-        <v>Min Response Time per DDI-first-architecture-go3</v>
+        <v>Min Response Time for DDI-first-architecture-go3</v>
       </c>
     </row>
     <row r="2">
@@ -763,17 +612,17 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Sat Sep 07 2024 18:35:42 GMT+0200 (Ora legale dell’Europa centrale)</v>
+        <v>Thu Sep 26 2024 01:03:21 GMT+0200 (Ora legale dell’Europa centrale)</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Sat Sep 07 2024 18:44:13 GMT+0200 (Ora legale dell’Europa centrale)</v>
+        <v>Thu Sep 26 2024 01:13:11 GMT+0200 (Ora legale dell’Europa centrale)</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Grain: Automatica</v>
+        <v>Grain: Automatic</v>
       </c>
     </row>
     <row r="6">
@@ -811,71 +660,71 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>45542.775</v>
+        <v>45561.044444444444</v>
       </c>
       <c r="B12">
-        <v>0.002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>45542.77569444444</v>
+        <v>45561.04513888889</v>
       </c>
       <c r="B13">
-        <v>0.021</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>45542.77638888889</v>
+        <v>45561.04583333333</v>
       </c>
       <c r="B14">
-        <v>0.027</v>
+        <v>0.028</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>45542.777083333334</v>
+        <v>45561.04652777778</v>
       </c>
       <c r="B15">
-        <v>0.028</v>
+        <v>0.027</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>45542.77777777778</v>
+        <v>45561.04722222222</v>
       </c>
       <c r="B16">
-        <v>0.013</v>
+        <v>0.009</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>45542.77847222222</v>
+        <v>45561.04791666667</v>
       </c>
       <c r="B17">
-        <v>0.029</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>45542.77916666667</v>
+        <v>45561.04861111111</v>
       </c>
       <c r="B18">
-        <v>0.039</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>45542.779861111114</v>
+        <v>45561.049305555556</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>45542.78055555555</v>
+        <v>45561.05</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -888,9 +737,160 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <cols>
+    <col min="1" max="1" customWidth="1" width="15"/>
+    <col min="2" max="2" customWidth="1" width="11"/>
+    <col min="3" max="3" customWidth="1" width="11"/>
+    <col min="4" max="4" customWidth="1" width="11"/>
+    <col min="5" max="5" customWidth="1" width="11"/>
+    <col min="6" max="6" customWidth="1" width="11"/>
+    <col min="7" max="7" customWidth="1" width="11"/>
+    <col min="8" max="8" customWidth="1" width="11"/>
+    <col min="9" max="9" customWidth="1" width="11"/>
+    <col min="10" max="10" customWidth="1" width="11"/>
+    <col min="11" max="11" customWidth="1" width="11"/>
+    <col min="12" max="12" customWidth="1" width="11"/>
+    <col min="13" max="13" customWidth="1" width="11"/>
+    <col min="14" max="14" customWidth="1" width="11"/>
+    <col min="15" max="15" customWidth="1" width="11"/>
+    <col min="16" max="16" customWidth="1" width="11"/>
+    <col min="17" max="17" customWidth="1" width="11"/>
+    <col min="18" max="18" customWidth="1" width="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v xml:space="preserve">Chart Title: </v>
+      </c>
+      <c r="B1" t="str">
+        <v>Avg Response Time for DDI-first-architecture-go3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Thu Sep 26 2024 01:03:21 GMT+0200 (Ora legale dell’Europa centrale)</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Thu Sep 26 2024 01:13:11 GMT+0200 (Ora legale dell’Europa centrale)</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Grain: Automatic</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Aggregation type: Avg</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Grouping: None</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Filters: None</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Chart type: Line</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v/>
+      </c>
+      <c r="B11" t="str">
+        <v>DDI-first-architecture-go3, Response Time (Avg), DDI-first-architecture-go3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1">
+        <v>45561.04513888889</v>
+      </c>
+      <c r="B12">
+        <v>0.1610625</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1">
+        <v>45561.04583333333</v>
+      </c>
+      <c r="B13">
+        <v>0.050076190476190476</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1">
+        <v>45561.04652777778</v>
+      </c>
+      <c r="B14">
+        <v>0.04663025210084034</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1">
+        <v>45561.04722222222</v>
+      </c>
+      <c r="B15">
+        <v>0.06258235294117648</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1">
+        <v>45561.04791666667</v>
+      </c>
+      <c r="B16">
+        <v>0.04234</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1">
+        <v>45561.04861111111</v>
+      </c>
+      <c r="B17">
+        <v>0.041743902439024386</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1">
+        <v>45561.049305555556</v>
+      </c>
+      <c r="B18">
+        <v>0.047</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:B18"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -915,6 +915,7 @@
     <col min="18" max="18" customWidth="1" width="11"/>
     <col min="19" max="19" customWidth="1" width="11"/>
     <col min="20" max="20" customWidth="1" width="11"/>
+    <col min="21" max="21" customWidth="1" width="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -922,7 +923,7 @@
         <v xml:space="preserve">Chart Title: </v>
       </c>
       <c r="B1" t="str">
-        <v>Max Response Time per DDI-first-architecture-go3</v>
+        <v>Max Response Time for DDI-first-architecture-go3</v>
       </c>
     </row>
     <row r="2">
@@ -932,17 +933,17 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Sat Sep 07 2024 18:35:42 GMT+0200 (Ora legale dell’Europa centrale)</v>
+        <v>Thu Sep 26 2024 01:03:21 GMT+0200 (Ora legale dell’Europa centrale)</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Sat Sep 07 2024 18:44:13 GMT+0200 (Ora legale dell’Europa centrale)</v>
+        <v>Thu Sep 26 2024 01:13:11 GMT+0200 (Ora legale dell’Europa centrale)</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>Grain: Automatica</v>
+        <v>Grain: Automatic</v>
       </c>
     </row>
     <row r="6">
@@ -980,79 +981,87 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>45542.775</v>
+        <v>45561.044444444444</v>
       </c>
       <c r="B12">
-        <v>0.022</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1">
-        <v>45542.77569444444</v>
+        <v>45561.04513888889</v>
       </c>
       <c r="B13">
-        <v>0.543</v>
+        <v>1.349</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1">
-        <v>45542.77638888889</v>
+        <v>45561.04583333333</v>
       </c>
       <c r="B14">
-        <v>0.412</v>
+        <v>0.701</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1">
-        <v>45542.777083333334</v>
+        <v>45561.04652777778</v>
       </c>
       <c r="B15">
-        <v>0.148</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1">
-        <v>45542.77777777778</v>
+        <v>45561.04722222222</v>
       </c>
       <c r="B16">
-        <v>0.901</v>
+        <v>0.861</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1">
-        <v>45542.77847222222</v>
+        <v>45561.04791666667</v>
       </c>
       <c r="B17">
-        <v>0.095</v>
+        <v>0.244</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1">
-        <v>45542.77916666667</v>
+        <v>45561.04861111111</v>
       </c>
       <c r="B18">
-        <v>0.08</v>
+        <v>0.084</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>45542.779861111114</v>
+        <v>45561.049305555556</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.085</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>45542.78055555555</v>
+        <v>45561.05</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21" s="1">
+        <v>45561.05069444444</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>